<commit_message>
Add QR code generation for specialists and implement search functionality in specialist management
</commit_message>
<xml_diff>
--- a/src/files/НОВЫЙ телефонный справочник 01.07.2025.xlsx
+++ b/src/files/НОВЫЙ телефонный справочник 01.07.2025.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\block\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\block\source\repos\gkznAnalytics\src\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC8D3B2-4FD2-41FC-881B-FB5EB0BFF161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6089D6E6-DDC0-48FF-9476-E2E4C5E85AF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="341">
   <si>
     <t>Должность</t>
   </si>
@@ -511,18 +511,12 @@
     <t>Представительство “ЦЗН Эвено-Бытантайского национального района” ГКУ РС(Я) "Центр занятости населения Республики Саха (Якутия)" 678580 РС(Я),Эвено-Бытантайский национальный улус, с.Батагай-Алыта, ул.Р.И.Шадрина, д.3</t>
   </si>
   <si>
-    <t>Представительство "ЦЗН Анабарского национального (долгано-эвенкийского) района ГКУ РС(Я) "Центр занятости населения Республики Саха (Якутия)" 678440 с.Саскылах ул.Октябрьская 12</t>
-  </si>
-  <si>
     <t>Представительство "ЦЗН Абыйского района" ГКУ РС(Я) "Центр занятости населения Республики Саха (Якутия)"678890, Абыйский улус, п. Белая Гора, ул. Ефимова, 1 +2 часа</t>
   </si>
   <si>
     <t>Представительство "ЦЗН Аллаиховского района" ГКУ РС(Я) "Центр занятости населения Республики Саха (Якутия)" 678880 п.Чокурдах ул. 50 лет СССР д.3</t>
   </si>
   <si>
-    <t>Представительство "ЦЗН Булунского района" ГКУ РС(Я) "Центр занятости населения Республики Саха (Якутия)" 678400 Тикси, ул. Академика Федорова 30</t>
-  </si>
-  <si>
     <t>Представительство "ЦЗН Верхнеколымского района" ГКУ РС(Я) "Центр занятости населения Республики Саха (Якутия)" п.Зырянка 678770 ул.Ленина 20 +2 час</t>
   </si>
   <si>
@@ -589,9 +583,6 @@
     <t>Филиал "ЦЗН Чурапчинского района" ГКУ РС(Я) "Центр занятости населения Республики Саха (Якутия)" 678670 с. Чурапча ул.Ленина 35а</t>
   </si>
   <si>
-    <t>Филиал "ЦЗН  Амгинского района" ГКУ РС(Я) "Центр занятости населения Республики Саха (Якутия)" 678600 с. Амга, ул Партизанская, д. 79</t>
-  </si>
-  <si>
     <t>Филиал "ЦЗН Верхоянского района" ГКУ РС(Я) "Центр занятости населения Республики Саха (Якутия)" 678500 Верхоянский район п. Батагай, ул. Ленина 16  +1 час</t>
   </si>
   <si>
@@ -1006,37 +997,7 @@
     <t>Отдел</t>
   </si>
   <si>
-    <t>Филиал "ЦЗН Алданского района" ГКУ РС(Я) "Центр занятости населения Республики Саха (Якутия)" 678900  г. Алдан ул. Ленина 10</t>
-  </si>
-  <si>
-    <t>Филиал "ЦЗН Алданского района" ГКУ РС(Я) "Центр занятости населения Республики Саха (Якутия)" 678900  г. Алдан ул. Ленина 11</t>
-  </si>
-  <si>
-    <t>Филиал "ЦЗН Алданского района" ГКУ РС(Я) "Центр занятости населения Республики Саха (Якутия)" 678900  г. Алдан ул. Ленина 12</t>
-  </si>
-  <si>
-    <t>Филиал "ЦЗН Алданского района" ГКУ РС(Я) "Центр занятости населения Республики Саха (Якутия)" 678900  г. Алдан ул. Ленина 13</t>
-  </si>
-  <si>
-    <t>Филиал "ЦЗН Алданского района" ГКУ РС(Я) "Центр занятости населения Республики Саха (Якутия)" 678900  г. Алдан ул. Ленина 14</t>
-  </si>
-  <si>
-    <t>Филиал "ЦЗН Алданского района" ГКУ РС(Я) "Центр занятости населения Республики Саха (Якутия)" 678900  г. Алдан ул. Ленина 15</t>
-  </si>
-  <si>
     <t>Филиал "ЦЗН  Амгинского района" ГКУ РС(Я) "Центр занятости населения Республики Саха (Якутия)" 678600 с. Амга, ул Партизанская, д. 78</t>
-  </si>
-  <si>
-    <t>Филиал "ЦЗН  Амгинского района" ГКУ РС(Я) "Центр занятости населения Республики Саха (Якутия)" 678600 с. Амга, ул Партизанская, д. 80</t>
-  </si>
-  <si>
-    <t>Филиал "ЦЗН  Амгинского района" ГКУ РС(Я) "Центр занятости населения Республики Саха (Якутия)" 678600 с. Амга, ул Партизанская, д. 81</t>
-  </si>
-  <si>
-    <t>Филиал "ЦЗН  Амгинского района" ГКУ РС(Я) "Центр занятости населения Республики Саха (Якутия)" 678600 с. Амга, ул Партизанская, д. 82</t>
-  </si>
-  <si>
-    <t>Филиал "ЦЗН  Амгинского района" ГКУ РС(Я) "Центр занятости населения Республики Саха (Якутия)" 678600 с. Амга, ул Партизанская, д. 83</t>
   </si>
   <si>
     <t>Представительство "ЦЗН Анабарского национального (долгано-эвенкийского) района ГКУ РС(Я) "Центр занятости населения Республики Саха (Якутия)" 678440 с.Саскылах ул.Октябрьская 11</t>
@@ -1552,8 +1513,8 @@
   </sheetPr>
   <dimension ref="A1:F245"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1569,10 +1530,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C1" s="15" t="s">
         <v>0</v>
@@ -1585,10 +1546,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>2</v>
@@ -1601,10 +1562,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>2</v>
@@ -1617,29 +1578,29 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C4" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>228</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>231</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>109</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>153</v>
@@ -1649,7 +1610,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>109</v>
@@ -1665,7 +1626,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>109</v>
@@ -1681,7 +1642,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>109</v>
@@ -1697,7 +1658,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>109</v>
@@ -1706,14 +1667,14 @@
         <v>17</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>109</v>
@@ -1722,14 +1683,14 @@
         <v>10</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>109</v>
@@ -1745,10 +1706,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>4</v>
@@ -1761,10 +1722,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>6</v>
@@ -1777,10 +1738,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>6</v>
@@ -1793,10 +1754,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>6</v>
@@ -1809,10 +1770,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>6</v>
@@ -1825,55 +1786,55 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>14</v>
@@ -1889,29 +1850,29 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>101</v>
@@ -1921,7 +1882,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>14</v>
@@ -1930,20 +1891,20 @@
         <v>99</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>107</v>
@@ -1953,23 +1914,23 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>14</v>
@@ -1978,17 +1939,17 @@
         <v>91</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>15</v>
@@ -2001,26 +1962,26 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>16</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>18</v>
@@ -2033,26 +1994,26 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>16</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>105</v>
@@ -2065,26 +2026,26 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
     </row>
     <row r="33" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>17</v>
@@ -2097,26 +2058,26 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>16</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>16</v>
@@ -2129,10 +2090,10 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>17</v>
@@ -2145,10 +2106,10 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>16</v>
@@ -2161,97 +2122,97 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D41" s="14" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
     </row>
     <row r="42" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B42" s="5"/>
       <c r="C42" s="7" t="s">
         <v>21</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="F42" s="2"/>
     </row>
     <row r="43" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B43" s="5"/>
       <c r="C43" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="F43" s="2"/>
     </row>
     <row r="44" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="7" t="s">
@@ -2265,103 +2226,103 @@
     </row>
     <row r="45" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>322</v>
+        <v>182</v>
       </c>
       <c r="B45" s="5"/>
       <c r="C45" s="7" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
     </row>
     <row r="46" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>323</v>
+        <v>182</v>
       </c>
       <c r="B46" s="5"/>
       <c r="C46" s="7" t="s">
         <v>98</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
     </row>
     <row r="47" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
-        <v>324</v>
+        <v>182</v>
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="7" t="s">
         <v>98</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
     </row>
     <row r="48" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
-        <v>325</v>
+        <v>182</v>
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="7" t="s">
         <v>98</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
     </row>
     <row r="49" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
-        <v>326</v>
+        <v>182</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="7" t="s">
         <v>97</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
     </row>
     <row r="50" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>327</v>
+        <v>182</v>
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="7" t="s">
         <v>97</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
     </row>
     <row r="51" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B51" s="5"/>
       <c r="C51" s="7" t="s">
         <v>21</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B52" s="5"/>
       <c r="C52" s="7" t="s">
@@ -2373,7 +2334,7 @@
     </row>
     <row r="53" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="B53" s="5"/>
       <c r="C53" s="7" t="s">
@@ -2385,7 +2346,7 @@
     </row>
     <row r="54" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
-        <v>183</v>
+        <v>319</v>
       </c>
       <c r="B54" s="5"/>
       <c r="C54" s="7" t="s">
@@ -2397,7 +2358,7 @@
     </row>
     <row r="55" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="B55" s="5"/>
       <c r="C55" s="7" t="s">
@@ -2409,7 +2370,7 @@
     </row>
     <row r="56" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
       <c r="B56" s="5"/>
       <c r="C56" s="7" t="s">
@@ -2421,7 +2382,7 @@
     </row>
     <row r="57" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
-        <v>331</v>
+        <v>319</v>
       </c>
       <c r="B57" s="5"/>
       <c r="C57" s="7" t="s">
@@ -2433,43 +2394,43 @@
     </row>
     <row r="58" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>332</v>
+        <v>319</v>
       </c>
       <c r="B58" s="5"/>
       <c r="C58" s="7" t="s">
         <v>16</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>333</v>
+        <v>320</v>
       </c>
       <c r="B59" s="5"/>
       <c r="C59" s="7" t="s">
         <v>121</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>157</v>
+        <v>320</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="7" t="s">
         <v>98</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>334</v>
+        <v>321</v>
       </c>
       <c r="B61" s="5"/>
       <c r="C61" s="7" t="s">
@@ -2481,19 +2442,19 @@
     </row>
     <row r="62" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>160</v>
+        <v>321</v>
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="7" t="s">
         <v>97</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B63" s="5"/>
       <c r="C63" s="7" t="s">
@@ -2505,7 +2466,7 @@
     </row>
     <row r="64" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B64" s="5"/>
       <c r="C64" s="7" t="s">
@@ -2517,7 +2478,7 @@
     </row>
     <row r="65" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B65" s="5"/>
       <c r="C65" s="7" t="s">
@@ -2529,19 +2490,19 @@
     </row>
     <row r="66" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B66" s="5"/>
       <c r="C66" s="7" t="s">
         <v>16</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B67" s="5"/>
       <c r="C67" s="7" t="s">
@@ -2553,19 +2514,19 @@
     </row>
     <row r="68" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B68" s="5"/>
       <c r="C68" s="7" t="s">
         <v>16</v>
       </c>
       <c r="D68" s="7" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B69" s="5"/>
       <c r="C69" s="7" t="s">
@@ -2577,7 +2538,7 @@
     </row>
     <row r="70" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B70" s="5"/>
       <c r="C70" s="7" t="s">
@@ -2589,31 +2550,31 @@
     </row>
     <row r="71" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B71" s="5"/>
       <c r="C71" s="7" t="s">
         <v>16</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B72" s="5"/>
       <c r="C72" s="7" t="s">
         <v>16</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B73" s="5"/>
       <c r="C73" s="7" t="s">
@@ -2625,7 +2586,7 @@
     </row>
     <row r="74" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B74" s="5"/>
       <c r="C74" s="7" t="s">
@@ -2637,7 +2598,7 @@
     </row>
     <row r="75" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B75" s="5"/>
       <c r="C75" s="10" t="s">
@@ -2649,19 +2610,19 @@
     </row>
     <row r="76" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B76" s="5"/>
       <c r="C76" s="7" t="s">
         <v>16</v>
       </c>
       <c r="D76" s="7" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B77" s="5"/>
       <c r="C77" s="7" t="s">
@@ -2673,7 +2634,7 @@
     </row>
     <row r="78" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B78" s="5"/>
       <c r="C78" s="7" t="s">
@@ -2685,7 +2646,7 @@
     </row>
     <row r="79" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B79" s="5"/>
       <c r="C79" s="7" t="s">
@@ -2697,7 +2658,7 @@
     </row>
     <row r="80" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B80" s="5"/>
       <c r="C80" s="7" t="s">
@@ -2709,7 +2670,7 @@
     </row>
     <row r="81" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B81" s="5"/>
       <c r="C81" s="7" t="s">
@@ -2721,7 +2682,7 @@
     </row>
     <row r="82" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B82" s="5"/>
       <c r="C82" s="7" t="s">
@@ -2733,7 +2694,7 @@
     </row>
     <row r="83" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B83" s="5"/>
       <c r="C83" s="7" t="s">
@@ -2745,7 +2706,7 @@
     </row>
     <row r="84" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B84" s="5"/>
       <c r="C84" s="7" t="s">
@@ -2757,7 +2718,7 @@
     </row>
     <row r="85" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B85" s="5"/>
       <c r="C85" s="7" t="s">
@@ -2769,43 +2730,43 @@
     </row>
     <row r="86" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B86" s="5"/>
       <c r="C86" s="7" t="s">
         <v>97</v>
       </c>
       <c r="D86" s="7" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B87" s="5"/>
       <c r="C87" s="7" t="s">
         <v>98</v>
       </c>
       <c r="D87" s="7" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B88" s="5"/>
       <c r="C88" s="7" t="s">
         <v>98</v>
       </c>
       <c r="D88" s="7" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B89" s="5"/>
       <c r="C89" s="7" t="s">
@@ -2817,7 +2778,7 @@
     </row>
     <row r="90" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B90" s="5"/>
       <c r="C90" s="7" t="s">
@@ -2829,7 +2790,7 @@
     </row>
     <row r="91" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B91" s="5"/>
       <c r="C91" s="7" t="s">
@@ -2841,19 +2802,19 @@
     </row>
     <row r="92" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B92" s="5"/>
       <c r="C92" s="7" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D92" s="11" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A93" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B93" s="5"/>
       <c r="C93" s="7" t="s">
@@ -2865,19 +2826,19 @@
     </row>
     <row r="94" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A94" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B94" s="5"/>
       <c r="C94" s="7" t="s">
         <v>97</v>
       </c>
       <c r="D94" s="11" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A95" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B95" s="5"/>
       <c r="C95" s="7" t="s">
@@ -2889,11 +2850,11 @@
     </row>
     <row r="96" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B96" s="5"/>
       <c r="C96" s="7" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D96" s="11" t="s">
         <v>47</v>
@@ -2901,7 +2862,7 @@
     </row>
     <row r="97" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A97" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B97" s="5"/>
       <c r="C97" s="7" t="s">
@@ -2913,7 +2874,7 @@
     </row>
     <row r="98" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A98" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B98" s="5"/>
       <c r="C98" s="7" t="s">
@@ -2925,31 +2886,31 @@
     </row>
     <row r="99" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B99" s="5"/>
       <c r="C99" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D99" s="7" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A100" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B100" s="5"/>
       <c r="C100" s="7" t="s">
         <v>98</v>
       </c>
       <c r="D100" s="7" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A101" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B101" s="5"/>
       <c r="C101" s="7" t="s">
@@ -2961,19 +2922,19 @@
     </row>
     <row r="102" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A102" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B102" s="5"/>
       <c r="C102" s="7" t="s">
         <v>124</v>
       </c>
       <c r="D102" s="7" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A103" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B103" s="5"/>
       <c r="C103" s="7" t="s">
@@ -2985,31 +2946,31 @@
     </row>
     <row r="104" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A104" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B104" s="5"/>
       <c r="C104" s="7" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D104" s="7" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A105" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B105" s="5"/>
       <c r="C105" s="7" t="s">
         <v>16</v>
       </c>
       <c r="D105" s="7" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B106" s="5"/>
       <c r="C106" s="7" t="s">
@@ -3021,31 +2982,31 @@
     </row>
     <row r="107" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A107" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B107" s="5"/>
       <c r="C107" s="7" t="s">
         <v>113</v>
       </c>
       <c r="D107" s="7" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A108" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B108" s="5"/>
       <c r="C108" s="7" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D108" s="7" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A109" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B109" s="5"/>
       <c r="C109" s="7" t="s">
@@ -3057,7 +3018,7 @@
     </row>
     <row r="110" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A110" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B110" s="5"/>
       <c r="C110" s="7" t="s">
@@ -3069,19 +3030,19 @@
     </row>
     <row r="111" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A111" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B111" s="5"/>
       <c r="C111" s="7" t="s">
         <v>16</v>
       </c>
       <c r="D111" s="7" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A112" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B112" s="5"/>
       <c r="C112" s="7" t="s">
@@ -3093,91 +3054,91 @@
     </row>
     <row r="113" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A113" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B113" s="5"/>
       <c r="C113" s="7" t="s">
         <v>16</v>
       </c>
       <c r="D113" s="7" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A114" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B114" s="5"/>
       <c r="C114" s="7" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D114" s="7" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A115" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B115" s="5"/>
       <c r="C115" s="7" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D115" s="7" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A116" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B116" s="5"/>
       <c r="C116" s="7" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D116" s="7" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A117" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B117" s="5"/>
       <c r="C117" s="7" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D117" s="7" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A118" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B118" s="5"/>
       <c r="C118" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D118" s="7" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A119" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B119" s="5"/>
       <c r="C119" s="7" t="s">
         <v>16</v>
       </c>
       <c r="D119" s="7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A120" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B120" s="5"/>
       <c r="C120" s="7" t="s">
@@ -3189,11 +3150,11 @@
     </row>
     <row r="121" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A121" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B121" s="5"/>
       <c r="C121" s="7" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D121" s="7" t="s">
         <v>52</v>
@@ -3201,31 +3162,31 @@
     </row>
     <row r="122" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A122" s="7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B122" s="5"/>
       <c r="C122" s="7" t="s">
         <v>113</v>
       </c>
       <c r="D122" s="5" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A123" s="7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B123" s="5"/>
       <c r="C123" s="7" t="s">
         <v>97</v>
       </c>
       <c r="D123" s="7" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A124" s="7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B124" s="5"/>
       <c r="C124" s="7" t="s">
@@ -3237,7 +3198,7 @@
     </row>
     <row r="125" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A125" s="7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B125" s="5"/>
       <c r="C125" s="7" t="s">
@@ -3249,7 +3210,7 @@
     </row>
     <row r="126" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A126" s="7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B126" s="5"/>
       <c r="C126" s="7" t="s">
@@ -3261,7 +3222,7 @@
     </row>
     <row r="127" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A127" s="7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B127" s="5"/>
       <c r="C127" s="7" t="s">
@@ -3273,7 +3234,7 @@
     </row>
     <row r="128" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A128" s="7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B128" s="5"/>
       <c r="C128" s="7" t="s">
@@ -3285,7 +3246,7 @@
     </row>
     <row r="129" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A129" s="7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B129" s="5"/>
       <c r="C129" s="7" t="s">
@@ -3297,7 +3258,7 @@
     </row>
     <row r="130" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A130" s="7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B130" s="5"/>
       <c r="C130" s="7" t="s">
@@ -3309,188 +3270,188 @@
     </row>
     <row r="131" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A131" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B131" s="5"/>
       <c r="C131" s="7" t="s">
         <v>113</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>348</v>
+        <v>335</v>
       </c>
       <c r="E131" s="13"/>
     </row>
     <row r="132" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A132" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B132" s="5"/>
       <c r="C132" s="7" t="s">
-        <v>349</v>
+        <v>336</v>
       </c>
       <c r="D132" s="5" t="s">
-        <v>347</v>
+        <v>334</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A133" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B133" s="5"/>
       <c r="C133" s="7" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="D133" s="5" t="s">
-        <v>346</v>
+        <v>333</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A134" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B134" s="5"/>
       <c r="C134" s="7" t="s">
-        <v>350</v>
+        <v>337</v>
       </c>
       <c r="D134" s="5" t="s">
-        <v>345</v>
+        <v>332</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A135" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B135" s="5"/>
       <c r="C135" s="7" t="s">
         <v>97</v>
       </c>
       <c r="D135" s="5" t="s">
-        <v>344</v>
+        <v>331</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A136" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B136" s="5"/>
       <c r="C136" s="7" t="s">
-        <v>351</v>
+        <v>338</v>
       </c>
       <c r="D136" s="5" t="s">
-        <v>343</v>
+        <v>330</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A137" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B137" s="5"/>
       <c r="C137" s="7" t="s">
         <v>97</v>
       </c>
       <c r="D137" s="5" t="s">
-        <v>342</v>
+        <v>329</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A138" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B138" s="5"/>
       <c r="C138" s="7" t="s">
         <v>97</v>
       </c>
       <c r="D138" s="5" t="s">
-        <v>341</v>
+        <v>328</v>
       </c>
     </row>
     <row r="139" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A139" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B139" s="5"/>
       <c r="C139" s="7" t="s">
         <v>97</v>
       </c>
       <c r="D139" s="5" t="s">
-        <v>340</v>
+        <v>327</v>
       </c>
     </row>
     <row r="140" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A140" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B140" s="5"/>
       <c r="C140" s="7" t="s">
         <v>97</v>
       </c>
       <c r="D140" s="5" t="s">
-        <v>339</v>
+        <v>326</v>
       </c>
     </row>
     <row r="141" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A141" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B141" s="5"/>
       <c r="C141" s="7" t="s">
         <v>122</v>
       </c>
       <c r="D141" s="5" t="s">
-        <v>338</v>
+        <v>325</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A142" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B142" s="5"/>
       <c r="C142" s="7" t="s">
-        <v>352</v>
+        <v>339</v>
       </c>
       <c r="D142" s="5" t="s">
-        <v>337</v>
+        <v>324</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A143" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B143" s="5"/>
       <c r="C143" s="7" t="s">
         <v>97</v>
       </c>
       <c r="D143" s="5" t="s">
-        <v>336</v>
+        <v>323</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A144" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B144" s="5"/>
       <c r="C144" s="7" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="D144" s="5" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="145" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A145" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B145" s="5"/>
       <c r="C145" s="7" t="s">
         <v>97</v>
       </c>
       <c r="D145" s="5" t="s">
-        <v>335</v>
+        <v>322</v>
       </c>
     </row>
     <row r="146" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A146" s="7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B146" s="5"/>
       <c r="C146" s="7" t="s">
@@ -3502,7 +3463,7 @@
     </row>
     <row r="147" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A147" s="7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B147" s="5"/>
       <c r="C147" s="7" t="s">
@@ -3514,7 +3475,7 @@
     </row>
     <row r="148" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A148" s="7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B148" s="5"/>
       <c r="C148" s="7" t="s">
@@ -3526,19 +3487,19 @@
     </row>
     <row r="149" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A149" s="7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B149" s="5"/>
       <c r="C149" s="7" t="s">
         <v>16</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="150" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A150" s="7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B150" s="5"/>
       <c r="C150" s="7" t="s">
@@ -3550,7 +3511,7 @@
     </row>
     <row r="151" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A151" s="7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B151" s="5"/>
       <c r="C151" s="7" t="s">
@@ -3562,7 +3523,7 @@
     </row>
     <row r="152" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A152" s="7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B152" s="5"/>
       <c r="C152" s="7" t="s">
@@ -3574,19 +3535,19 @@
     </row>
     <row r="153" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A153" s="7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B153" s="5"/>
       <c r="C153" s="7" t="s">
         <v>98</v>
       </c>
       <c r="D153" s="4" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="154" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A154" s="7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B154" s="5"/>
       <c r="C154" s="7" t="s">
@@ -3598,19 +3559,19 @@
     </row>
     <row r="155" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A155" s="7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B155" s="5"/>
       <c r="C155" s="7" t="s">
         <v>98</v>
       </c>
       <c r="D155" s="4" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="156" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A156" s="7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B156" s="5"/>
       <c r="C156" s="7" t="s">
@@ -3629,7 +3590,7 @@
         <v>113</v>
       </c>
       <c r="D157" s="4" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="158" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
@@ -3641,7 +3602,7 @@
         <v>97</v>
       </c>
       <c r="D158" s="4" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="159" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
@@ -3653,7 +3614,7 @@
         <v>98</v>
       </c>
       <c r="D159" s="4" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="160" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
@@ -3665,7 +3626,7 @@
         <v>98</v>
       </c>
       <c r="D160" s="4" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="161" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
@@ -3677,12 +3638,12 @@
         <v>98</v>
       </c>
       <c r="D161" s="4" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="162" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A162" s="7" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B162" s="5"/>
       <c r="C162" s="7" t="s">
@@ -3694,31 +3655,31 @@
     </row>
     <row r="163" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A163" s="7" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B163" s="5"/>
       <c r="C163" s="7" t="s">
         <v>97</v>
       </c>
       <c r="D163" s="4" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="164" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A164" s="7" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B164" s="5"/>
       <c r="C164" s="7" t="s">
         <v>98</v>
       </c>
       <c r="D164" s="4" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="165" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A165" s="7" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B165" s="5"/>
       <c r="C165" s="7" t="s">
@@ -3730,19 +3691,19 @@
     </row>
     <row r="166" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A166" s="7" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B166" s="5"/>
       <c r="C166" s="7" t="s">
         <v>98</v>
       </c>
       <c r="D166" s="4" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="167" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A167" s="7" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B167" s="5"/>
       <c r="C167" s="7" t="s">
@@ -3754,19 +3715,19 @@
     </row>
     <row r="168" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A168" s="7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B168" s="5"/>
       <c r="C168" s="7" t="s">
         <v>113</v>
       </c>
       <c r="D168" s="4" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="169" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A169" s="7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B169" s="5"/>
       <c r="C169" s="7" t="s">
@@ -3778,7 +3739,7 @@
     </row>
     <row r="170" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A170" s="7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B170" s="5"/>
       <c r="C170" s="7" t="s">
@@ -3790,7 +3751,7 @@
     </row>
     <row r="171" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A171" s="7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B171" s="5"/>
       <c r="C171" s="7" t="s">
@@ -3802,7 +3763,7 @@
     </row>
     <row r="172" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A172" s="7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B172" s="5"/>
       <c r="C172" s="7" t="s">
@@ -3814,19 +3775,19 @@
     </row>
     <row r="173" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A173" s="7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B173" s="5"/>
       <c r="C173" s="7" t="s">
         <v>98</v>
       </c>
       <c r="D173" s="4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="174" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A174" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B174" s="5"/>
       <c r="C174" s="7" t="s">
@@ -3838,7 +3799,7 @@
     </row>
     <row r="175" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A175" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B175" s="5"/>
       <c r="C175" s="7" t="s">
@@ -3850,19 +3811,19 @@
     </row>
     <row r="176" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A176" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B176" s="5"/>
       <c r="C176" s="7" t="s">
         <v>97</v>
       </c>
       <c r="D176" s="4" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="177" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A177" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B177" s="5"/>
       <c r="C177" s="7" t="s">
@@ -3874,7 +3835,7 @@
     </row>
     <row r="178" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A178" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B178" s="5"/>
       <c r="C178" s="7" t="s">
@@ -3886,7 +3847,7 @@
     </row>
     <row r="179" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A179" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B179" s="5"/>
       <c r="C179" s="7" t="s">
@@ -3898,7 +3859,7 @@
     </row>
     <row r="180" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A180" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B180" s="5"/>
       <c r="C180" s="7" t="s">
@@ -3910,7 +3871,7 @@
     </row>
     <row r="181" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A181" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B181" s="5"/>
       <c r="C181" s="7" t="s">
@@ -3922,7 +3883,7 @@
     </row>
     <row r="182" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A182" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B182" s="5"/>
       <c r="C182" s="7" t="s">
@@ -3934,7 +3895,7 @@
     </row>
     <row r="183" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A183" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B183" s="5"/>
       <c r="C183" s="7" t="s">
@@ -3946,7 +3907,7 @@
     </row>
     <row r="184" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A184" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B184" s="5"/>
       <c r="C184" s="7" t="s">
@@ -3958,7 +3919,7 @@
     </row>
     <row r="185" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A185" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B185" s="5"/>
       <c r="C185" s="7" t="s">
@@ -3970,19 +3931,19 @@
     </row>
     <row r="186" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A186" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B186" s="5"/>
       <c r="C186" s="7" t="s">
         <v>98</v>
       </c>
       <c r="D186" s="4" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="187" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A187" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B187" s="5"/>
       <c r="C187" s="7" t="s">
@@ -3994,7 +3955,7 @@
     </row>
     <row r="188" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A188" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B188" s="5"/>
       <c r="C188" s="7" t="s">
@@ -4006,7 +3967,7 @@
     </row>
     <row r="189" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A189" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B189" s="5"/>
       <c r="C189" s="7" t="s">
@@ -4018,7 +3979,7 @@
     </row>
     <row r="190" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A190" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B190" s="5"/>
       <c r="C190" s="7" t="s">
@@ -4030,19 +3991,19 @@
     </row>
     <row r="191" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A191" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B191" s="5"/>
       <c r="C191" s="7" t="s">
         <v>97</v>
       </c>
       <c r="D191" s="4" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="192" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A192" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B192" s="5"/>
       <c r="C192" s="7" t="s">
@@ -4054,43 +4015,43 @@
     </row>
     <row r="193" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A193" s="7" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B193" s="5"/>
       <c r="C193" s="7" t="s">
         <v>121</v>
       </c>
       <c r="D193" s="4" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="194" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A194" s="7" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B194" s="5"/>
       <c r="C194" s="7" t="s">
         <v>97</v>
       </c>
       <c r="D194" s="3" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="195" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A195" s="7" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B195" s="5"/>
       <c r="C195" s="7" t="s">
         <v>98</v>
       </c>
       <c r="D195" s="3" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="196" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A196" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B196" s="5"/>
       <c r="C196" s="7" t="s">
@@ -4102,7 +4063,7 @@
     </row>
     <row r="197" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A197" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B197" s="5"/>
       <c r="C197" s="7" t="s">
@@ -4114,7 +4075,7 @@
     </row>
     <row r="198" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A198" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B198" s="5"/>
       <c r="C198" s="7" t="s">
@@ -4126,7 +4087,7 @@
     </row>
     <row r="199" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A199" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B199" s="5"/>
       <c r="C199" s="7" t="s">
@@ -4138,7 +4099,7 @@
     </row>
     <row r="200" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A200" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B200" s="5"/>
       <c r="C200" s="7" t="s">
@@ -4150,31 +4111,31 @@
     </row>
     <row r="201" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A201" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B201" s="5"/>
       <c r="C201" s="7" t="s">
         <v>98</v>
       </c>
       <c r="D201" s="3" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="202" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A202" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B202" s="5"/>
       <c r="C202" s="7" t="s">
         <v>98</v>
       </c>
       <c r="D202" s="3" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="203" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A203" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B203" s="5"/>
       <c r="C203" s="7" t="s">
@@ -4186,7 +4147,7 @@
     </row>
     <row r="204" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A204" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B204" s="5"/>
       <c r="C204" s="7" t="s">
@@ -4198,7 +4159,7 @@
     </row>
     <row r="205" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A205" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B205" s="5"/>
       <c r="C205" s="7" t="s">
@@ -4210,7 +4171,7 @@
     </row>
     <row r="206" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A206" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B206" s="5"/>
       <c r="C206" s="7" t="s">
@@ -4222,19 +4183,19 @@
     </row>
     <row r="207" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A207" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B207" s="5"/>
       <c r="C207" s="7" t="s">
         <v>98</v>
       </c>
       <c r="D207" s="3" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="208" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A208" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B208" s="5"/>
       <c r="C208" s="7" t="s">
@@ -4246,14 +4207,14 @@
     </row>
     <row r="209" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A209" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B209" s="5"/>
       <c r="C209" s="7" t="s">
         <v>97</v>
       </c>
       <c r="D209" s="3" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="210" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
@@ -4277,12 +4238,12 @@
         <v>98</v>
       </c>
       <c r="D211" s="3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" s="7" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="B212" s="4" t="s">
         <v>134</v>
@@ -4296,7 +4257,7 @@
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" s="7" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="B213" s="4" t="s">
         <v>134</v>
@@ -4310,7 +4271,7 @@
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" s="7" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="B214" s="4" t="s">
         <v>136</v>
@@ -4324,7 +4285,7 @@
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" s="7" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="B215" s="4" t="s">
         <v>136</v>
@@ -4333,12 +4294,12 @@
         <v>148</v>
       </c>
       <c r="D215" s="4" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" s="7" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="B216" s="4" t="s">
         <v>136</v>
@@ -4347,12 +4308,12 @@
         <v>16</v>
       </c>
       <c r="D216" s="4" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" s="7" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="B217" s="4" t="s">
         <v>136</v>
@@ -4366,7 +4327,7 @@
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" s="7" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="B218" s="4" t="s">
         <v>136</v>
@@ -4375,12 +4336,12 @@
         <v>16</v>
       </c>
       <c r="D218" s="4" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" s="7" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="B219" s="4" t="s">
         <v>136</v>
@@ -4389,12 +4350,12 @@
         <v>16</v>
       </c>
       <c r="D219" s="4" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" s="7" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="B220" s="4" t="s">
         <v>136</v>
@@ -4403,12 +4364,12 @@
         <v>16</v>
       </c>
       <c r="D220" s="4" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" s="7" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="B221" s="4" t="s">
         <v>136</v>
@@ -4417,12 +4378,12 @@
         <v>16</v>
       </c>
       <c r="D221" s="4" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" s="7" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="B222" s="4" t="s">
         <v>136</v>
@@ -4431,12 +4392,12 @@
         <v>16</v>
       </c>
       <c r="D222" s="4" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" s="7" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="B223" s="4" t="s">
         <v>136</v>
@@ -4445,12 +4406,12 @@
         <v>16</v>
       </c>
       <c r="D223" s="5" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" s="7" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="B224" s="4" t="s">
         <v>138</v>
@@ -4464,13 +4425,13 @@
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" s="7" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="B225" s="4" t="s">
         <v>138</v>
       </c>
       <c r="C225" s="4" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D225" s="4" t="s">
         <v>139</v>
@@ -4478,7 +4439,7 @@
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" s="7" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="B226" s="4" t="s">
         <v>138</v>
@@ -4492,7 +4453,7 @@
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" s="7" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="B227" s="4" t="s">
         <v>138</v>
@@ -4506,7 +4467,7 @@
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" s="7" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="B228" s="4" t="s">
         <v>138</v>
@@ -4515,12 +4476,12 @@
         <v>16</v>
       </c>
       <c r="D228" s="4" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" s="7" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="B229" s="4" t="s">
         <v>138</v>
@@ -4529,12 +4490,12 @@
         <v>16</v>
       </c>
       <c r="D229" s="4" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" s="7" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="B230" s="4" t="s">
         <v>138</v>
@@ -4548,7 +4509,7 @@
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" s="7" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="B231" s="4" t="s">
         <v>138</v>
@@ -4557,12 +4518,12 @@
         <v>16</v>
       </c>
       <c r="D231" s="4" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" s="7" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="B232" s="4" t="s">
         <v>138</v>
@@ -4571,85 +4532,85 @@
         <v>16</v>
       </c>
       <c r="D232" s="4" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" s="7" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="B233" s="4" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C233" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D233" s="4" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" s="7" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="B234" s="4" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C234" s="4" t="s">
         <v>93</v>
       </c>
       <c r="D234" s="4" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" s="7" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="B235" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="C235" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="C235" s="4" t="s">
-        <v>309</v>
-      </c>
       <c r="D235" s="4" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" s="7" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="B236" s="4" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C236" s="4" t="s">
         <v>93</v>
       </c>
       <c r="D236" s="4" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" s="7" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="B237" s="4" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C237" s="4" t="s">
         <v>93</v>
       </c>
       <c r="D237" s="5" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" s="7" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="B238" s="4" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C238" s="4" t="s">
         <v>15</v>
@@ -4660,80 +4621,80 @@
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" s="7" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="B239" s="4" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C239" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D239" s="4" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" s="7" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="B240" s="4" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C240" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D240" s="4" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" s="7" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="B241" s="4" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C241" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D241" s="4" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" s="7" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="B242" s="4" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C242" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D242" s="4" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" s="7" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="B243" s="4" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C243" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D243" s="4" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" s="7" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="B244" s="4" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C244" s="4" t="s">
         <v>17</v>
@@ -4744,16 +4705,16 @@
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" s="7" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="B245" s="4" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C245" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D245" s="4" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
   </sheetData>

</xml_diff>